<commit_message>
1st working excel version
</commit_message>
<xml_diff>
--- a/Radiator Database.xlsx
+++ b/Radiator Database.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\phili\Documents\GitSourceCode\Radiators\radiators2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BD446A0-3937-47A5-B7D7-14DC7DFD118F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35DCF6A3-061A-401F-A4C5-E191195540E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19838" windowHeight="12780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="43200" yWindow="0" windowWidth="44235" windowHeight="25380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RadiatorDatabase" sheetId="2" r:id="rId1"/>

</xml_diff>